<commit_message>
Add more for recursive
</commit_message>
<xml_diff>
--- a/题目汇总.xlsx
+++ b/题目汇总.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="1039">
   <si>
     <t xml:space="preserve">题目</t>
   </si>
@@ -7794,6 +7794,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">时直接输出</t>
     </r>
@@ -7813,6 +7814,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，其余的数输出（</t>
     </r>
@@ -7832,6 +7834,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">。只有一个</t>
     </r>
@@ -7851,6 +7854,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">时，一刀不用。偶数个人时，切</t>
     </r>
@@ -7870,6 +7874,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">刀；奇数个人时（</t>
     </r>
@@ -7889,6 +7894,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -7908,6 +7914,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">刀。</t>
     </r>
@@ -17024,6 +17031,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">反向思考：给定一个长度分割的次数最多。分割的方法是：最短</t>
     </r>
@@ -17043,6 +17051,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">、剩余两根相差</t>
     </r>
@@ -17062,6 +17071,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">。这样就能够得出递推公式：</t>
     </r>
@@ -17081,8 +17091,266 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">。注意数据类型的选择！！</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/CF103A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">对于每一道题目有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ai</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">个选项因此会</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ai-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">次错误。假设之前选了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">f[i-1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">次，第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">题选错总共选了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">f[i-1]+i*(ai-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">次，第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">题最后选对一共选了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">f[i-1]+i*(ai-1)+i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">次</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/CF509A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">首先初始化首行首列，然后依据题意填充矩阵，填充的过程中记录最大值。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/AT_tenka1_2012_qualA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">简单递推斐波那起数列</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/AT_abc006_2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">按题目描述递推，注意计算过程中需要模</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">10007</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/P1176</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">两张表，一张描述障碍物的分布，一张统计步数。如果某格子上有障碍物，就不更新步数；如果没有障碍物则</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">f[i][j]=f[i-1][j]+f[i][j-1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，到达左侧和上边的步数之和。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.luogu.com.cn/problem/P1644</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">从起点开始</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">dfs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，直到最后一点。</t>
     </r>
   </si>
   <si>
@@ -18574,7 +18842,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -18695,12 +18963,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
@@ -18799,6 +19061,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -19001,10 +19276,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -19033,19 +19304,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -19055,6 +19326,10 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -19145,9 +19420,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>671400</xdr:colOff>
+      <xdr:colOff>670680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>4939200</xdr:rowOff>
+      <xdr:rowOff>4938480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -19161,7 +19436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11461320" y="3098880"/>
-          <a:ext cx="8514000" cy="4913640"/>
+          <a:ext cx="8513280" cy="4912920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19504,7 +19779,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -19580,7 +19855,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>464</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -19705,7 +19980,7 @@
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>475</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -19757,10 +20032,10 @@
       <c r="A10" s="0" t="s">
         <v>487</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>488</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>489</v>
       </c>
     </row>
@@ -19779,7 +20054,7 @@
       <c r="B12" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>494</v>
       </c>
     </row>
@@ -19926,7 +20201,7 @@
       <c r="A29" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>529</v>
       </c>
     </row>
@@ -19975,7 +20250,7 @@
       <c r="A35" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="28" t="s">
         <v>541</v>
       </c>
       <c r="C35" s="4"/>
@@ -20303,7 +20578,7 @@
       <c r="A74" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B74" s="27" t="s">
         <v>617</v>
       </c>
     </row>
@@ -20493,7 +20768,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="30" t="s">
+      <c r="A97" s="29" t="s">
         <v>661</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -20655,7 +20930,7 @@
       <c r="A116" s="0" t="s">
         <v>699</v>
       </c>
-      <c r="B116" s="31" t="s">
+      <c r="B116" s="30" t="s">
         <v>700</v>
       </c>
       <c r="C116" s="4"/>
@@ -20761,7 +21036,7 @@
       <c r="A129" s="0" t="s">
         <v>725</v>
       </c>
-      <c r="B129" s="32" t="s">
+      <c r="B129" s="31" t="s">
         <v>726</v>
       </c>
     </row>
@@ -20793,7 +21068,7 @@
       <c r="A133" s="0" t="s">
         <v>733</v>
       </c>
-      <c r="B133" s="28" t="s">
+      <c r="B133" s="27" t="s">
         <v>734</v>
       </c>
     </row>
@@ -21243,7 +21518,7 @@
       <c r="A18" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>815</v>
       </c>
       <c r="C18" s="4"/>
@@ -21587,7 +21862,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -21743,7 +22018,7 @@
       <c r="A19" s="2" t="s">
         <v>806</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>894</v>
       </c>
     </row>
@@ -21980,7 +22255,7 @@
       <c r="A14" s="0" t="s">
         <v>930</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>931</v>
       </c>
     </row>
@@ -22024,10 +22299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22137,13 +22412,62 @@
       <c r="A13" s="0" t="s">
         <v>957</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="3" t="s">
         <v>958</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>961</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>967</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>969</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="https://www.luogu.com.cn/problem/P1164"/>
+    <hyperlink ref="A19" r:id="rId2" display="https://www.luogu.com.cn/problem/P1644"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -22377,7 +22701,7 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>959</v>
+        <v>971</v>
       </c>
     </row>
   </sheetData>
@@ -22456,10 +22780,10 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>960</v>
+        <v>972</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>961</v>
+        <v>973</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22467,94 +22791,94 @@
         <v>823</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>962</v>
+        <v>974</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>963</v>
+        <v>975</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>964</v>
+        <v>976</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>965</v>
+        <v>977</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>966</v>
+        <v>978</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>967</v>
+        <v>979</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>968</v>
+        <v>980</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>969</v>
+        <v>981</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>970</v>
+        <v>982</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>972</v>
+        <v>984</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>976</v>
+        <v>988</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>979</v>
+        <v>991</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>980</v>
+        <v>992</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>981</v>
+        <v>993</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>983</v>
+        <v>995</v>
       </c>
     </row>
   </sheetData>
@@ -22606,103 +22930,103 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>984</v>
+        <v>996</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>985</v>
+        <v>997</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>986</v>
+        <v>998</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>988</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>989</v>
+        <v>1001</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>990</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>993</v>
+        <v>1005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>994</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>995</v>
+        <v>1007</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>996</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>997</v>
+        <v>1009</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>998</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>999</v>
+        <v>1011</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>1000</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1001</v>
+        <v>1013</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1002</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1003</v>
+        <v>1015</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1004</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1005</v>
+        <v>1017</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1006</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1007</v>
+        <v>1019</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1008</v>
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -22748,74 +23072,74 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1009</v>
+        <v>1021</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1010</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>1011</v>
+        <v>1023</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1012</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>1013</v>
+        <v>1025</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1014</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1015</v>
+        <v>1027</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1016</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1017</v>
+        <v>1029</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1018</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1019</v>
+        <v>1031</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1020</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1021</v>
+        <v>1033</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1022</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>1023</v>
+        <v>1035</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1024</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>1025</v>
+        <v>1037</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1026</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>
@@ -23188,10 +23512,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23281,6 +23605,8 @@
       </c>
       <c r="C9" s="4"/>
     </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.luogu.com.cn/problem/P1428"/>
@@ -24820,7 +25146,7 @@
       <c r="A67" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="3" t="s">
         <v>440</v>
       </c>
     </row>
@@ -24958,7 +25284,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>451</v>
       </c>
       <c r="B7" s="3" t="s">

</xml_diff>